<commit_message>
atualizado a lista de jogos ps3
</commit_message>
<xml_diff>
--- a/Lista Jogos PS3.xlsx
+++ b/Lista Jogos PS3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Valid</t>
   </si>
@@ -132,10 +132,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -160,72 +160,108 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -237,45 +273,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -290,15 +298,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -319,43 +319,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -373,133 +493,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -513,17 +513,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -543,35 +546,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -596,17 +581,32 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -615,157 +615,154 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1107,7 +1104,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelCol="4"/>
@@ -1118,17 +1115,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1"/>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1138,7 +1135,7 @@
       </c>
     </row>
     <row r="3" ht="21" spans="2:5">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3">
@@ -1146,87 +1143,93 @@
       </c>
       <c r="E3">
         <f>SUM(C2:C40)</f>
-        <v>197.81</v>
+        <v>149.74</v>
       </c>
     </row>
     <row r="4" ht="21" spans="2:3">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4">
         <v>11.76</v>
       </c>
     </row>
-    <row r="5" ht="21" spans="1:3">
+    <row r="5" ht="21" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>1.9</v>
       </c>
     </row>
-    <row r="6" ht="21" spans="2:3">
-      <c r="B6" s="3" t="s">
+    <row r="6" ht="21" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>9.84</v>
       </c>
     </row>
-    <row r="7" ht="21" spans="1:3">
+    <row r="7" ht="21" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>3.9</v>
       </c>
     </row>
     <row r="8" ht="21" spans="2:3">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C8">
         <v>8.9</v>
       </c>
     </row>
-    <row r="9" ht="21" spans="1:3">
-      <c r="A9" s="2" t="s">
+    <row r="9" ht="21" spans="1:4">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>7.4</v>
       </c>
     </row>
-    <row r="10" ht="21" spans="1:3">
+    <row r="10" ht="21" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>7.36</v>
       </c>
     </row>
-    <row r="11" ht="21" spans="2:3">
-      <c r="B11" s="3" t="s">
+    <row r="11" ht="21" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>11.27</v>
       </c>
     </row>
     <row r="12" ht="21" spans="2:3">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C12">
@@ -1234,7 +1237,7 @@
       </c>
     </row>
     <row r="13" ht="21" spans="2:3">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C13">
@@ -1242,7 +1245,7 @@
       </c>
     </row>
     <row r="14" ht="21" spans="2:3">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C14">
@@ -1250,7 +1253,7 @@
       </c>
     </row>
     <row r="15" ht="21" spans="2:3">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C15">
@@ -1258,16 +1261,16 @@
       </c>
     </row>
     <row r="16" ht="21" spans="2:4">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4">
         <v>18.15</v>
       </c>
     </row>
     <row r="17" ht="21" spans="2:3">
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C17">
@@ -1275,7 +1278,7 @@
       </c>
     </row>
     <row r="18" ht="21" spans="2:3">
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C18">
@@ -1283,7 +1286,7 @@
       </c>
     </row>
     <row r="19" ht="21" spans="2:3">
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C19">
@@ -1291,25 +1294,25 @@
       </c>
     </row>
     <row r="20" ht="21" spans="2:4">
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5">
+      <c r="C20" s="4"/>
+      <c r="D20" s="4">
         <v>34.02</v>
       </c>
     </row>
     <row r="21" ht="21" spans="2:4">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5">
+      <c r="C21" s="4"/>
+      <c r="D21" s="4">
         <v>10.13</v>
       </c>
     </row>
     <row r="22" ht="21" spans="2:3">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C22">
@@ -1317,7 +1320,7 @@
       </c>
     </row>
     <row r="23" ht="21" spans="2:3">
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C23">
@@ -1325,16 +1328,16 @@
       </c>
     </row>
     <row r="24" ht="21" spans="2:4">
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="25" ht="21" spans="2:3">
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C25">
@@ -1342,16 +1345,16 @@
       </c>
     </row>
     <row r="26" ht="21" spans="2:4">
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5">
+      <c r="C26" s="4"/>
+      <c r="D26" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="27" ht="21" spans="2:3">
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C27">
@@ -1359,32 +1362,33 @@
       </c>
     </row>
     <row r="28" ht="21" spans="2:3">
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C28">
         <v>3.3</v>
       </c>
     </row>
-    <row r="29" ht="21" spans="2:3">
+    <row r="29" ht="21" spans="2:4">
       <c r="B29" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="4"/>
+      <c r="D29" s="4">
         <v>6.4</v>
       </c>
     </row>
     <row r="30" ht="21" spans="2:4">
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5">
+      <c r="C30" s="4"/>
+      <c r="D30" s="4">
         <v>6.51</v>
       </c>
     </row>
     <row r="31" ht="21" spans="2:3">
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C31">
@@ -1392,7 +1396,7 @@
       </c>
     </row>
     <row r="32" ht="21" spans="2:3">
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C32">
@@ -1400,11 +1404,11 @@
       </c>
     </row>
     <row r="33" ht="21" spans="2:4">
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5">
+      <c r="C33" s="4"/>
+      <c r="D33" s="4">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado lista de jogos ps3
</commit_message>
<xml_diff>
--- a/Lista Jogos PS3.xlsx
+++ b/Lista Jogos PS3.xlsx
@@ -13,17 +13,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1556071360" val="944" rev="123" revOS="3"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1556071360" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1556071360" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1556071360"/>
+      <pm:revision xmlns:pm="smNativeData" day="1557192364" val="944" rev="123" revOS="3"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1557192364" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1557192364" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1557192364"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Valid</t>
   </si>
@@ -163,7 +163,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1556071360" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557192364" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -178,7 +178,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1556071360" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557192364" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -194,7 +194,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1556071360" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557192364" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -204,12 +204,11 @@
     </font>
     <font>
       <name val="Proxima Nova"/>
-      <charset val="134"/>
       <color rgb="FF333333"/>
       <sz val="15"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1556071360" fgClr="333333" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557192364" fgClr="333333" ulstyle="none" kern="1">
             <pm:latin face="Proxima Nova" sz="300" lang="default"/>
             <pm:cs face="Basic Roman" sz="300" lang="default"/>
             <pm:ea face="Basic Roman" sz="300" lang="default"/>
@@ -224,7 +223,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1556071360" fgClr="FFFFFF" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557192364" fgClr="FFFFFF" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -240,7 +239,7 @@
       <sz val="13"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1556071360" fgClr="44546A" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557192364" fgClr="44546A" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="260" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="260" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="260" lang="default" weight="bold"/>
@@ -256,7 +255,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1556071360" fgClr="800080" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557192364" fgClr="800080" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -272,7 +271,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1556071360" fgClr="44546A" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557192364" fgClr="44546A" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -287,7 +286,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1556071360" fgClr="006100" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557192364" fgClr="006100" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -303,7 +302,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1556071360" fgClr="FA7D00" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557192364" fgClr="FA7D00" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -319,7 +318,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1556071360" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557192364" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -335,7 +334,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1556071360" fgClr="3F3F3F" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557192364" fgClr="3F3F3F" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -350,7 +349,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1556071360" fgClr="9C0006" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557192364" fgClr="9C0006" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -365,7 +364,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1556071360" fgClr="FF0000" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557192364" fgClr="FF0000" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -380,7 +379,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1556071360" fgClr="9C6500" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557192364" fgClr="9C6500" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -395,7 +394,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1556071360" fgClr="FA7D00" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557192364" fgClr="FA7D00" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -411,7 +410,7 @@
       <sz val="15"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1556071360" fgClr="44546A" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557192364" fgClr="44546A" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="300" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="300" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="300" lang="default" weight="bold"/>
@@ -427,7 +426,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1556071360" fgClr="7F7F7F" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557192364" fgClr="7F7F7F" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" i="1"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" i="1"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" i="1"/>
@@ -443,7 +442,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1556071360" fgClr="FFFFFF" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557192364" fgClr="FFFFFF" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -459,7 +458,7 @@
       <sz val="18"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1556071360" fgClr="44546A" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557192364" fgClr="44546A" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="360" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="360" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="360" lang="default" weight="bold"/>
@@ -474,7 +473,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1556071360" fgClr="3F3F76" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557192364" fgClr="3F3F76" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -496,7 +495,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00A8D08C" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00A8D08C" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -507,7 +506,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00C5DFB3" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00C5DFB3" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -518,7 +517,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="008EA9DB" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="008EA9DB" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -529,7 +528,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="0070AD47" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="0070AD47" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -540,7 +539,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00B4C6E7" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00B4C6E7" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -551,7 +550,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00D9E1F2" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00D9E1F2" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -562,7 +561,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00FFD964" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00FFD964" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -573,7 +572,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="004472C4" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="004472C4" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -584,7 +583,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00FFE697" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00FFE697" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -595,7 +594,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00FFC000" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00FFC000" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -609,7 +608,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00D9D9D9" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00D9D9D9" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -620,7 +619,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00F4AF82" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00F4AF82" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -631,7 +630,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -642,7 +641,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00F8CAAB" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00F8CAAB" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -653,7 +652,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00FBE3D5" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00FBE3D5" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -664,7 +663,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00ED7D31" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00ED7D31" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -675,7 +674,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00BDD7EE" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00BDD7EE" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -686,7 +685,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00DDEBF7" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00DDEBF7" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -697,7 +696,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="005B9BD5" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="005B9BD5" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -708,7 +707,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00FFEB9C" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00FFEB9C" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -719,7 +718,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="009BC2E6" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="009BC2E6" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -730,7 +729,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00FFC7CE" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00FFC7CE" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -741,7 +740,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00FFF2CA" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00FFF2CA" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -755,7 +754,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00F2F2F2" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00F2F2F2" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -766,7 +765,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00EBEBEB" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00EBEBEB" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -777,7 +776,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -788,7 +787,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00FFCC99" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00FFCC99" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -799,7 +798,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00F2F2F2" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00F2F2F2" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -810,7 +809,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00C6EFCE" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00C6EFCE" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -827,7 +826,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00E1EFD8" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00E1EFD8" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -838,7 +837,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -849,7 +848,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00C7C7C7" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00C7C7C7" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -860,7 +859,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1556071360" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557192364" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -882,197 +881,197 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
         </ext>
       </extLst>
     </border>
@@ -1091,7 +1090,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360">
+          <pm:border xmlns:pm="smNativeData" id="1557192364">
             <pm:line position="bottom" type="2" style="0" width="20" dist="20" width2="20" rgb="FF8001"/>
           </pm:border>
         </ext>
@@ -1112,235 +1111,235 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
         </ext>
       </extLst>
     </border>
@@ -1359,7 +1358,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360">
+          <pm:border xmlns:pm="smNativeData" id="1557192364">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="5B9BD5"/>
             <pm:line position="bottom" type="2" style="0" width="20" dist="20" width2="20" rgb="5B9BD5"/>
           </pm:border>
@@ -1381,7 +1380,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360">
+          <pm:border xmlns:pm="smNativeData" id="1557192364">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
@@ -1405,7 +1404,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
         </ext>
       </extLst>
     </border>
@@ -1424,7 +1423,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360">
+          <pm:border xmlns:pm="smNativeData" id="1557192364">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
@@ -1448,7 +1447,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360">
+          <pm:border xmlns:pm="smNativeData" id="1557192364">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
@@ -1472,7 +1471,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360">
+          <pm:border xmlns:pm="smNativeData" id="1557192364">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
@@ -1496,7 +1495,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
         </ext>
       </extLst>
     </border>
@@ -1515,7 +1514,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360">
+          <pm:border xmlns:pm="smNativeData" id="1557192364">
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="ACCCEA"/>
           </pm:border>
         </ext>
@@ -1536,7 +1535,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360">
+          <pm:border xmlns:pm="smNativeData" id="1557192364">
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="5B9BD5"/>
           </pm:border>
         </ext>
@@ -1557,7 +1556,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
         </ext>
       </extLst>
     </border>
@@ -1576,7 +1575,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360">
+          <pm:border xmlns:pm="smNativeData" id="1557192364">
             <pm:line position="top" type="2" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
             <pm:line position="bottom" type="2" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
             <pm:line position="left" type="2" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
@@ -1600,26 +1599,26 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1556071360"/>
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1557192364"/>
         </ext>
       </extLst>
     </border>
@@ -1937,7 +1936,7 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:cellMargin xmlns:pm="smNativeData" id="1556071360" l="192" r="0" t="0" b="0" textRotation="0"/>
+          <pm:cellMargin xmlns:pm="smNativeData" id="1557192364" l="192" r="0" t="0" b="0" textRotation="0"/>
         </ext>
       </extLst>
     </xf>
@@ -1999,10 +1998,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1556071360" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1557192364" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1556071360" count="41">
+      <pm:colors xmlns:pm="smNativeData" id="1557192364" count="41">
         <pm:color name="Cor 24" rgb="44546A"/>
         <pm:color name="Cor 25" rgb="800080"/>
         <pm:color name="Cor 26" rgb="006100"/>
@@ -2280,12 +2279,12 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
   <cols>
-    <col min="1" max="1" width="8.803571" style="49"/>
+    <col min="1" max="1" width="8.803571" customWidth="1" style="49"/>
     <col min="2" max="2" width="42.401786" customWidth="1"/>
     <col min="3" max="3" width="13.098214" customWidth="1"/>
   </cols>
@@ -2319,7 +2318,7 @@
       </c>
       <c r="E3">
         <f>SUM(C2:C40)</f>
-        <v>136.849999999999994</v>
+        <v>113.230000000000004</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -2370,7 +2369,6 @@
       <c r="B8" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="C8"/>
       <c r="D8" t="n">
         <v>8.90000000000000036</v>
       </c>
@@ -2431,16 +2429,19 @@
       <c r="B14" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C14"/>
       <c r="D14" t="n">
         <v>3.99000000000000021</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="1:4">
+      <c r="A15" s="49" t="s">
+        <v>7</v>
+      </c>
       <c r="B15" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15"/>
+      <c r="D15" t="n">
         <v>3.5</v>
       </c>
     </row>
@@ -2571,19 +2572,26 @@
         <v>6.50999999999999979</v>
       </c>
     </row>
-    <row r="31" spans="2:3">
+    <row r="31" spans="1:4">
+      <c r="A31" s="49" t="s">
+        <v>7</v>
+      </c>
       <c r="B31" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="C31" t="n">
+      <c r="C31"/>
+      <c r="D31" t="n">
         <v>7.40000000000000036</v>
       </c>
     </row>
-    <row r="32" spans="2:3">
+    <row r="32" spans="1:4">
+      <c r="A32" s="49" t="s">
+        <v>7</v>
+      </c>
       <c r="B32" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="C32" t="n">
+      <c r="D32" t="n">
         <v>12.7200000000000006</v>
       </c>
     </row>
@@ -2600,7 +2608,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1556071360" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1557192364" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2609,14 +2617,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1556071360" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1556071360" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1557192364" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1557192364" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1556071360" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1557192364" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
atualizado lista de jogos ps3, incluido imagens hp e arquivos de exrcicios vue
</commit_message>
<xml_diff>
--- a/Lista Jogos PS3.xlsx
+++ b/Lista Jogos PS3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cezar T Nakase\projetos\projetos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cezar\projetos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Valid</t>
   </si>
@@ -147,8 +147,8 @@
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="173" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -900,7 +900,7 @@
     <xf numFmtId="0" fontId="10" fillId="27" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="28" borderId="27" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -939,7 +939,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1400,7 +1400,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="E3">
         <f>SUM(C2:C40)</f>
-        <v>103.03</v>
+        <v>93.45</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18.75">
@@ -1536,10 +1536,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="18.75">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>9.58</v>
       </c>
     </row>

</xml_diff>